<commit_message>
Updated the permissions reports for the data and application schemas
</commit_message>
<xml_diff>
--- a/CRDMA/docs/CEN_CRUISE_APP_permissions.xlsx
+++ b/CRDMA/docs/CEN_CRUISE_APP_permissions.xlsx
@@ -20,308 +20,338 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="114">
+  <si>
+    <t>Role Name</t>
+  </si>
   <si>
     <t>Owner Schema</t>
   </si>
   <si>
-    <t>Object Type</t>
-  </si>
-  <si>
     <t>Object Name</t>
   </si>
   <si>
     <t>Granted Privileges</t>
   </si>
   <si>
+    <t>Grant Option?</t>
+  </si>
+  <si>
+    <t>CAS_EXT_APP_ROLE</t>
+  </si>
+  <si>
+    <t>CAS</t>
+  </si>
+  <si>
+    <t>CAS_EXT_AUTH_PKG</t>
+  </si>
+  <si>
+    <t>EXECUTE</t>
+  </si>
+  <si>
+    <t>CCD_APP_ROLE</t>
+  </si>
+  <si>
     <t>CEN_CRUISE</t>
   </si>
   <si>
-    <t>PACKAGE</t>
-  </si>
-  <si>
-    <t>AUTH_APP_PKG</t>
-  </si>
-  <si>
-    <t>EXECUTE</t>
+    <t>AFF_RESPONSES</t>
+  </si>
+  <si>
+    <t>INSERT, SELECT</t>
+  </si>
+  <si>
+    <t>AFF_RESPONSES_V</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>AFF_RESP_TYPES</t>
+  </si>
+  <si>
+    <t>CCD_CRUISES</t>
+  </si>
+  <si>
+    <t>DELETE, INSERT, SELECT, UPDATE</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_AGG_V</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_EXP_SPP</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_ISS_SUMM_V</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_LEGS</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_LEG_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_LEG_V</t>
   </si>
   <si>
     <t>CCD_CRUISE_PKG</t>
   </si>
   <si>
+    <t>CCD_CRUISE_SPP_ESA</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_SPP_FSSI</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_SPP_MMPA</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_SUMM_ISS_V</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_SUMM_V</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_SVY_CATS</t>
+  </si>
+  <si>
+    <t>CCD_CRUISE_V</t>
+  </si>
+  <si>
+    <t>CCD_DATA_SETS</t>
+  </si>
+  <si>
+    <t>CCD_DATA_SETS_V</t>
+  </si>
+  <si>
+    <t>CCD_DATA_SET_STATUS</t>
+  </si>
+  <si>
+    <t>CCD_DATA_SET_TYPES</t>
+  </si>
+  <si>
     <t>CCD_DVM_PKG</t>
   </si>
   <si>
+    <t>CCD_EXP_SPP_CATS</t>
+  </si>
+  <si>
+    <t>CCD_GEAR</t>
+  </si>
+  <si>
+    <t>CCD_GEAR_PRE</t>
+  </si>
+  <si>
+    <t>CCD_GEAR_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_GEAR_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_GEAR_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_LEG_ALIASES</t>
+  </si>
+  <si>
+    <t>CCD_LEG_DATA_SETS</t>
+  </si>
+  <si>
+    <t>CCD_LEG_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_LEG_ECOSYSTEMS</t>
+  </si>
+  <si>
+    <t>CCD_LEG_GEAR</t>
+  </si>
+  <si>
+    <t>CCD_LEG_REGIONS</t>
+  </si>
+  <si>
+    <t>CCD_LEG_V</t>
+  </si>
+  <si>
+    <t>CCD_PLAT_TYPES</t>
+  </si>
+  <si>
+    <t>CCD_QC_LEG_OVERLAP_V</t>
+  </si>
+  <si>
+    <t>CCD_REGIONS</t>
+  </si>
+  <si>
+    <t>CCD_REGION_PRE</t>
+  </si>
+  <si>
+    <t>CCD_REGION_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_REGION_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_REGION_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_REG_ECOSYSTEMS</t>
+  </si>
+  <si>
+    <t>CCD_REG_ECO_PRE</t>
+  </si>
+  <si>
+    <t>CCD_REG_ECO_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_REG_ECO_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_REG_ECO_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_SCI_CENTERS</t>
+  </si>
+  <si>
+    <t>CCD_SCI_CENTER_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_SCI_CENTER_DIVS</t>
+  </si>
+  <si>
+    <t>CCD_SCI_CENTER_DIV_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_CAT_PRE</t>
+  </si>
+  <si>
+    <t>CCD_SPP_CAT_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_CAT_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_SPP_CAT_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_ESA_PRE</t>
+  </si>
+  <si>
+    <t>CCD_SPP_ESA_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_ESA_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_SPP_ESA_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_FSSI_PRE</t>
+  </si>
+  <si>
+    <t>CCD_SPP_FSSI_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_FSSI_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_SPP_FSSI_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_MMPA_PRE</t>
+  </si>
+  <si>
+    <t>CCD_SPP_MMPA_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_SPP_MMPA_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_SPP_MMPA_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_STD_SVY_NAMES</t>
+  </si>
+  <si>
+    <t>CCD_SVY_CATS</t>
+  </si>
+  <si>
+    <t>CCD_SVY_CAT_PRE</t>
+  </si>
+  <si>
+    <t>CCD_SVY_CAT_PRE_DELIM_V</t>
+  </si>
+  <si>
+    <t>CCD_SVY_CAT_PRE_OPTS</t>
+  </si>
+  <si>
+    <t>CCD_SVY_CAT_PRE_V</t>
+  </si>
+  <si>
+    <t>CCD_SVY_FREQ</t>
+  </si>
+  <si>
+    <t>CCD_SVY_TYPES</t>
+  </si>
+  <si>
+    <t>CCD_TGT_SPP_ESA</t>
+  </si>
+  <si>
+    <t>CCD_TGT_SPP_FSSI</t>
+  </si>
+  <si>
+    <t>CCD_TGT_SPP_MMPA</t>
+  </si>
+  <si>
+    <t>CCD_TGT_SPP_OTHER</t>
+  </si>
+  <si>
+    <t>CCD_VESSELS</t>
+  </si>
+  <si>
+    <t>CC_CONFIG_OPTIONS</t>
+  </si>
+  <si>
     <t>CUST_ERR_PKG</t>
   </si>
   <si>
     <t>DB_LOG_PKG</t>
   </si>
   <si>
+    <t>DVM_ISSUES</t>
+  </si>
+  <si>
+    <t>DELETE, SELECT, UPDATE</t>
+  </si>
+  <si>
+    <t>DVM_ISS_RES_TYPES</t>
+  </si>
+  <si>
+    <t>DVM_ISS_SEVERITY</t>
+  </si>
+  <si>
+    <t>DVM_ISS_TYPES</t>
+  </si>
+  <si>
+    <t>DVM_ISS_TYP_ASSOC</t>
+  </si>
+  <si>
+    <t>DELETE, SELECT</t>
+  </si>
+  <si>
     <t>DVM_PKG</t>
   </si>
   <si>
-    <t>TABLE</t>
-  </si>
-  <si>
-    <t>CCD_CRUISES</t>
-  </si>
-  <si>
-    <t>DELETE, INSERT, SELECT, UPDATE</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_EXP_SPP</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_LEGS</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_SPP_ESA</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_SPP_FSSI</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_SPP_MMPA</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_SVY_CATS</t>
-  </si>
-  <si>
-    <t>CCD_EXP_SPP_CATS</t>
-  </si>
-  <si>
-    <t>CCD_GEAR</t>
-  </si>
-  <si>
-    <t>CCD_GEAR_PRE</t>
-  </si>
-  <si>
-    <t>CCD_GEAR_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_LEG_ALIASES</t>
-  </si>
-  <si>
-    <t>CCD_LEG_ECOSYSTEMS</t>
-  </si>
-  <si>
-    <t>CCD_LEG_GEAR</t>
-  </si>
-  <si>
-    <t>CCD_LEG_REGIONS</t>
-  </si>
-  <si>
-    <t>CCD_PLAT_TYPES</t>
-  </si>
-  <si>
-    <t>CCD_REGIONS</t>
-  </si>
-  <si>
-    <t>CCD_REGION_PRE</t>
-  </si>
-  <si>
-    <t>CCD_REGION_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_REG_ECOSYSTEMS</t>
-  </si>
-  <si>
-    <t>CCD_REG_ECO_PRE</t>
-  </si>
-  <si>
-    <t>CCD_REG_ECO_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_SCI_CENTERS</t>
-  </si>
-  <si>
-    <t>CCD_SCI_CENTER_DIVS</t>
-  </si>
-  <si>
-    <t>CCD_SPP_CAT_PRE</t>
-  </si>
-  <si>
-    <t>CCD_SPP_CAT_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_SPP_ESA_PRE</t>
-  </si>
-  <si>
-    <t>CCD_SPP_ESA_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_SPP_FSSI_PRE</t>
-  </si>
-  <si>
-    <t>CCD_SPP_FSSI_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_SPP_MMPA_PRE</t>
-  </si>
-  <si>
-    <t>CCD_SPP_MMPA_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_STD_SVY_NAMES</t>
-  </si>
-  <si>
-    <t>CCD_SVY_CATS</t>
-  </si>
-  <si>
-    <t>CCD_SVY_CAT_PRE</t>
-  </si>
-  <si>
-    <t>CCD_SVY_CAT_PRE_OPTS</t>
-  </si>
-  <si>
-    <t>CCD_SVY_FREQ</t>
-  </si>
-  <si>
-    <t>CCD_SVY_TYPES</t>
-  </si>
-  <si>
-    <t>CCD_TGT_SPP_ESA</t>
-  </si>
-  <si>
-    <t>CCD_TGT_SPP_FSSI</t>
-  </si>
-  <si>
-    <t>CCD_TGT_SPP_MMPA</t>
-  </si>
-  <si>
-    <t>CCD_TGT_SPP_OTHER</t>
-  </si>
-  <si>
-    <t>CCD_VESSELS</t>
-  </si>
-  <si>
-    <t>DVM_ISSUES</t>
-  </si>
-  <si>
-    <t>DELETE, SELECT, UPDATE</t>
-  </si>
-  <si>
-    <t>DVM_ISS_RES_TYPES</t>
-  </si>
-  <si>
-    <t>SELECT</t>
-  </si>
-  <si>
-    <t>DVM_ISS_SEVERITY</t>
-  </si>
-  <si>
-    <t>DVM_ISS_TYPES</t>
-  </si>
-  <si>
-    <t>DVM_ISS_TYP_ASSOC</t>
-  </si>
-  <si>
-    <t>DELETE, SELECT</t>
-  </si>
-  <si>
     <t>DVM_PTA_ISSUES</t>
   </si>
   <si>
-    <t>VIEW</t>
-  </si>
-  <si>
-    <t>AUTH_APP_USERS_V</t>
-  </si>
-  <si>
-    <t>AUTH_APP_USER_GROUPS_V</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_ISS_SUMM_V</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_LEGS_V</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_LEG_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_SUMM_ISS_V</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_SUMM_V</t>
-  </si>
-  <si>
-    <t>CCD_CRUISE_V</t>
-  </si>
-  <si>
-    <t>CCD_DATA_SETS_V</t>
-  </si>
-  <si>
-    <t>CCD_GEAR_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_GEAR_PRE_V</t>
-  </si>
-  <si>
-    <t>CCD_LEG_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_LEG_V</t>
-  </si>
-  <si>
-    <t>CCD_QC_LEG_OVERLAP_V</t>
-  </si>
-  <si>
-    <t>CCD_REGION_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_REGION_PRE_V</t>
-  </si>
-  <si>
-    <t>CCD_REG_ECO_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_REG_ECO_PRE_V</t>
-  </si>
-  <si>
-    <t>CCD_SCI_CENTER_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_SCI_CENTER_DIV_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_CAT_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_CAT_PRE_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_ESA_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_ESA_PRE_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_FSSI_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_FSSI_PRE_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_MMPA_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_SPP_MMPA_PRE_V</t>
-  </si>
-  <si>
-    <t>CCD_SVY_CAT_PRE_DELIM_V</t>
-  </si>
-  <si>
-    <t>CCD_SVY_CAT_PRE_V</t>
-  </si>
-  <si>
     <t>DVM_PTA_ISSUES_V</t>
   </si>
   <si>
+    <t>CEN_UTILS_ROLE</t>
+  </si>
+  <si>
     <t>CEN_UTILS</t>
   </si>
   <si>
@@ -331,13 +361,14 @@
     <t>CEN_UTIL_PKG</t>
   </si>
   <si>
-    <t>select user_tab_privs.owner "Owner Schema", all_objects.object_type "Object Type", user_tab_privs.table_name "Object Name", LISTAGG(PRIVILEGE, ', ') WITHIN GROUP (ORDER BY PRIVILEGE) as "Granted Privileges" from user_tab_privs 
-inner join all_objects ON user_tab_privs.table_name = all_objects.object_name 
-AND all_objects.owner = user_tab_privs.owner
-AND all_objects.object_type &lt;&gt; 'PACKAGE BODY'
-where GRANTEE = sys_context( 'userenv', 'current_schema' )
-group by user_tab_privs.owner, user_tab_privs.table_name, all_objects.object_type
-order by user_tab_privs.owner, all_objects.object_type, table_name</t>
+    <t>(select ROLE "Role Name", OWNER "Owner Schema", TABLE_NAME "Object Name", LISTAGG(PRIVILEGE, ', ') WITHIN GROUP (ORDER BY PRIVILEGE) "Granted Privileges", NULL "Grant Option?" from role_tab_privs
+group by ROLE, OWNER, TABLE_NAME
+UNION 
+SELECT distinct NULL "Role Name", OWNER "Owner Schema", TABLE_NAME "Object Name", LISTAGG(PRIVILEGE, ', ') WITHIN GROUP (ORDER BY PRIVILEGE) "Granted Privileges", GRANTABLE "Grant Option?"
+from user_tab_privs 
+WHERE GRANTEE = sys_context( 'userenv', 'current_schema' )
+group by OWNER, TABLE_NAME, GRANTABLE)
+ORDER BY 1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -658,19 +689,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B89" sqref="B89"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,1251 +717,1352 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D48" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D55" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s">
         <v>68</v>
       </c>
       <c r="D57" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C58" t="s">
         <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C59" t="s">
         <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C60" t="s">
         <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
         <v>72</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
         <v>73</v>
       </c>
       <c r="D62" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C63" t="s">
         <v>74</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C64" t="s">
         <v>75</v>
       </c>
       <c r="D64" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C65" t="s">
         <v>76</v>
       </c>
       <c r="D65" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C66" t="s">
         <v>77</v>
       </c>
       <c r="D66" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C67" t="s">
         <v>78</v>
       </c>
       <c r="D67" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C68" t="s">
         <v>79</v>
       </c>
       <c r="D68" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C69" t="s">
         <v>80</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C70" t="s">
         <v>81</v>
       </c>
       <c r="D70" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
         <v>82</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C72" t="s">
         <v>83</v>
       </c>
       <c r="D72" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C73" t="s">
         <v>84</v>
       </c>
       <c r="D73" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C74" t="s">
         <v>85</v>
       </c>
       <c r="D74" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C75" t="s">
         <v>86</v>
       </c>
       <c r="D75" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C76" t="s">
         <v>87</v>
       </c>
       <c r="D76" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C77" t="s">
         <v>88</v>
       </c>
       <c r="D77" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B78" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
         <v>89</v>
       </c>
       <c r="D78" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C79" t="s">
         <v>90</v>
       </c>
       <c r="D79" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C80" t="s">
         <v>91</v>
       </c>
       <c r="D80" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C81" t="s">
         <v>92</v>
       </c>
       <c r="D81" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C82" t="s">
         <v>93</v>
       </c>
       <c r="D82" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C83" t="s">
         <v>94</v>
       </c>
       <c r="D83" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C84" t="s">
         <v>95</v>
       </c>
       <c r="D84" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C85" t="s">
         <v>96</v>
       </c>
       <c r="D85" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C86" t="s">
         <v>97</v>
       </c>
       <c r="D86" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C87" t="s">
         <v>98</v>
       </c>
       <c r="D87" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C88" t="s">
         <v>99</v>
       </c>
       <c r="D88" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C89" t="s">
         <v>101</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C90" t="s">
         <v>102</v>
       </c>
       <c r="D90" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" t="s">
+        <v>103</v>
+      </c>
+      <c r="D91" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" t="s">
+        <v>104</v>
+      </c>
+      <c r="D92" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" t="s">
+        <v>106</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" t="s">
+        <v>107</v>
+      </c>
+      <c r="D94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" t="s">
+        <v>108</v>
+      </c>
+      <c r="D95" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>109</v>
+      </c>
+      <c r="B97" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97" t="s">
+        <v>112</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1945,7 +2080,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>